<commit_message>
Refactor eavl_fpr_latency: complete function extraction from function
</commit_message>
<xml_diff>
--- a/data/dos_mqtt_iot/models/xgb/results/0.0005_all.xlsx
+++ b/data/dos_mqtt_iot/models/xgb/results/0.0005_all.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="53">
   <si>
     <t>start_idx_attack</t>
   </si>
@@ -44,13 +44,13 @@
     <t>attack_type</t>
   </si>
   <si>
-    <t>fpr</t>
-  </si>
-  <si>
     <t>pr</t>
   </si>
   <si>
     <t>rec</t>
+  </si>
+  <si>
+    <t>fpr</t>
   </si>
   <si>
     <t>tn</t>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>detected</t>
-  </si>
-  <si>
-    <t>29063697000 nanoseconds</t>
   </si>
   <si>
     <t>BF1_DDoS_AD</t>
@@ -190,7 +187,7 @@
 97    0.0005
 98    0.0005
 99    0.0005
-Name: target_fpr, Length: 100, dtype: object</t>
+Name: target_fpr, Length: 100, dtype: float64</t>
   </si>
 </sst>
 </file>
@@ -615,11 +612,11 @@
       <c r="B2">
         <v>35538</v>
       </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
+      <c r="C2" s="2">
+        <v>0.0003363853819444445</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.0003363853819444445</v>
       </c>
       <c r="E2">
         <v>35538</v>
@@ -631,12 +628,12 @@
         <v>8145</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
         <v>0</v>
       </c>
       <c r="L2">
@@ -681,12 +678,12 @@
         <v>17324</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
         <v>0</v>
       </c>
       <c r="L3">
@@ -731,12 +728,12 @@
         <v>15881</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
@@ -781,12 +778,12 @@
         <v>12026</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
         <v>0</v>
       </c>
       <c r="L5">
@@ -831,12 +828,12 @@
         <v>7540</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
         <v>0</v>
       </c>
       <c r="L6">
@@ -881,12 +878,12 @@
         <v>26163</v>
       </c>
       <c r="H7" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
       </c>
       <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
         <v>0</v>
       </c>
       <c r="L7">
@@ -931,12 +928,12 @@
         <v>2278</v>
       </c>
       <c r="H8" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
         <v>0</v>
       </c>
       <c r="L8">
@@ -981,12 +978,12 @@
         <v>4803</v>
       </c>
       <c r="H9" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
       </c>
       <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
         <v>0</v>
       </c>
       <c r="L9">
@@ -1031,12 +1028,12 @@
         <v>7719</v>
       </c>
       <c r="H10" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
       </c>
       <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
@@ -1081,12 +1078,12 @@
         <v>24635</v>
       </c>
       <c r="H11" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
       </c>
       <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
         <v>0</v>
       </c>
       <c r="L11">
@@ -1131,12 +1128,12 @@
         <v>19165</v>
       </c>
       <c r="H12" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
       </c>
       <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
         <v>0</v>
       </c>
       <c r="L12">
@@ -1181,12 +1178,12 @@
         <v>17269</v>
       </c>
       <c r="H13" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
       </c>
       <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
         <v>0</v>
       </c>
       <c r="L13">
@@ -1231,12 +1228,12 @@
         <v>23752</v>
       </c>
       <c r="H14" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
       </c>
       <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
         <v>0</v>
       </c>
       <c r="L14">
@@ -1281,12 +1278,12 @@
         <v>20186</v>
       </c>
       <c r="H15" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
       </c>
       <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
         <v>0</v>
       </c>
       <c r="L15">
@@ -1331,12 +1328,12 @@
         <v>28005</v>
       </c>
       <c r="H16" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
       </c>
       <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
         <v>0</v>
       </c>
       <c r="L16">
@@ -1381,12 +1378,12 @@
         <v>23874</v>
       </c>
       <c r="H17" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
       </c>
       <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
@@ -1431,12 +1428,12 @@
         <v>1510</v>
       </c>
       <c r="H18" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
       </c>
       <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
         <v>0</v>
       </c>
       <c r="L18">
@@ -1481,12 +1478,12 @@
         <v>4705</v>
       </c>
       <c r="H19" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
       </c>
       <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19">
         <v>0</v>
       </c>
       <c r="L19">
@@ -1531,12 +1528,12 @@
         <v>11947</v>
       </c>
       <c r="H20" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
       </c>
       <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
         <v>0</v>
       </c>
       <c r="L20">
@@ -1581,12 +1578,12 @@
         <v>7888</v>
       </c>
       <c r="H21" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
       </c>
       <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
         <v>0</v>
       </c>
       <c r="L21">
@@ -1631,12 +1628,12 @@
         <v>11076</v>
       </c>
       <c r="H22" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
       </c>
       <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
         <v>0</v>
       </c>
       <c r="L22">
@@ -1681,12 +1678,12 @@
         <v>13118</v>
       </c>
       <c r="H23" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
       </c>
       <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
         <v>0</v>
       </c>
       <c r="L23">
@@ -1731,12 +1728,12 @@
         <v>12375</v>
       </c>
       <c r="H24" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
       </c>
       <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24">
         <v>0</v>
       </c>
       <c r="L24">
@@ -1781,12 +1778,12 @@
         <v>5607</v>
       </c>
       <c r="H25" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
       </c>
       <c r="J25">
-        <v>0</v>
-      </c>
-      <c r="K25">
         <v>0</v>
       </c>
       <c r="L25">
@@ -1831,12 +1828,12 @@
         <v>11777</v>
       </c>
       <c r="H26" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
       </c>
       <c r="J26">
-        <v>0</v>
-      </c>
-      <c r="K26">
         <v>0</v>
       </c>
       <c r="L26">
@@ -1881,12 +1878,12 @@
         <v>10367</v>
       </c>
       <c r="H27" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
       </c>
       <c r="J27">
-        <v>0</v>
-      </c>
-      <c r="K27">
         <v>0</v>
       </c>
       <c r="L27">
@@ -1931,12 +1928,12 @@
         <v>6247</v>
       </c>
       <c r="H28" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
       </c>
       <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="K28">
         <v>0</v>
       </c>
       <c r="L28">
@@ -1981,12 +1978,12 @@
         <v>5284</v>
       </c>
       <c r="H29" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
       </c>
       <c r="J29">
-        <v>0</v>
-      </c>
-      <c r="K29">
         <v>0</v>
       </c>
       <c r="L29">
@@ -2031,12 +2028,12 @@
         <v>4651</v>
       </c>
       <c r="H30" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
       </c>
       <c r="J30">
-        <v>0</v>
-      </c>
-      <c r="K30">
         <v>0</v>
       </c>
       <c r="L30">
@@ -2081,12 +2078,12 @@
         <v>11716</v>
       </c>
       <c r="H31" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
       </c>
       <c r="J31">
-        <v>0</v>
-      </c>
-      <c r="K31">
         <v>0</v>
       </c>
       <c r="L31">
@@ -2131,12 +2128,12 @@
         <v>8384</v>
       </c>
       <c r="H32" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
       </c>
       <c r="J32">
-        <v>0</v>
-      </c>
-      <c r="K32">
         <v>0</v>
       </c>
       <c r="L32">
@@ -2181,12 +2178,12 @@
         <v>11582</v>
       </c>
       <c r="H33" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
       </c>
       <c r="J33">
-        <v>0</v>
-      </c>
-      <c r="K33">
         <v>0</v>
       </c>
       <c r="L33">
@@ -2231,12 +2228,12 @@
         <v>5919</v>
       </c>
       <c r="H34" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
       </c>
       <c r="J34">
-        <v>0</v>
-      </c>
-      <c r="K34">
         <v>0</v>
       </c>
       <c r="L34">
@@ -2281,12 +2278,12 @@
         <v>9098</v>
       </c>
       <c r="H35" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
       </c>
       <c r="J35">
-        <v>0</v>
-      </c>
-      <c r="K35">
         <v>0</v>
       </c>
       <c r="L35">
@@ -2331,12 +2328,12 @@
         <v>2289</v>
       </c>
       <c r="H36" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
       </c>
       <c r="J36">
-        <v>0</v>
-      </c>
-      <c r="K36">
         <v>0</v>
       </c>
       <c r="L36">
@@ -2381,12 +2378,12 @@
         <v>2073</v>
       </c>
       <c r="H37" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
       </c>
       <c r="J37">
-        <v>0</v>
-      </c>
-      <c r="K37">
         <v>0</v>
       </c>
       <c r="L37">
@@ -2431,12 +2428,12 @@
         <v>1823</v>
       </c>
       <c r="H38" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
       </c>
       <c r="J38">
-        <v>0</v>
-      </c>
-      <c r="K38">
         <v>0</v>
       </c>
       <c r="L38">
@@ -2481,12 +2478,12 @@
         <v>4098</v>
       </c>
       <c r="H39" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
       </c>
       <c r="J39">
-        <v>0</v>
-      </c>
-      <c r="K39">
         <v>0</v>
       </c>
       <c r="L39">
@@ -2531,12 +2528,12 @@
         <v>3480</v>
       </c>
       <c r="H40" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
       </c>
       <c r="J40">
-        <v>0</v>
-      </c>
-      <c r="K40">
         <v>0</v>
       </c>
       <c r="L40">
@@ -2581,12 +2578,12 @@
         <v>2446</v>
       </c>
       <c r="H41" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
       </c>
       <c r="J41">
-        <v>0</v>
-      </c>
-      <c r="K41">
         <v>0</v>
       </c>
       <c r="L41">
@@ -2631,12 +2628,12 @@
         <v>1626</v>
       </c>
       <c r="H42" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
       </c>
       <c r="J42">
-        <v>0</v>
-      </c>
-      <c r="K42">
         <v>0</v>
       </c>
       <c r="L42">
@@ -2681,12 +2678,12 @@
         <v>3040</v>
       </c>
       <c r="H43" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
       </c>
       <c r="J43">
-        <v>0</v>
-      </c>
-      <c r="K43">
         <v>0</v>
       </c>
       <c r="L43">
@@ -2731,12 +2728,12 @@
         <v>3455</v>
       </c>
       <c r="H44" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
       </c>
       <c r="J44">
-        <v>0</v>
-      </c>
-      <c r="K44">
         <v>0</v>
       </c>
       <c r="L44">
@@ -2781,12 +2778,12 @@
         <v>3678</v>
       </c>
       <c r="H45" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
       </c>
       <c r="J45">
-        <v>0</v>
-      </c>
-      <c r="K45">
         <v>0</v>
       </c>
       <c r="L45">
@@ -2831,12 +2828,12 @@
         <v>2846</v>
       </c>
       <c r="H46" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
       </c>
       <c r="J46">
-        <v>0</v>
-      </c>
-      <c r="K46">
         <v>0</v>
       </c>
       <c r="L46">
@@ -2881,12 +2878,12 @@
         <v>1957</v>
       </c>
       <c r="H47" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
       </c>
       <c r="J47">
-        <v>0</v>
-      </c>
-      <c r="K47">
         <v>0</v>
       </c>
       <c r="L47">
@@ -2931,12 +2928,12 @@
         <v>3904</v>
       </c>
       <c r="H48" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
       </c>
       <c r="J48">
-        <v>0</v>
-      </c>
-      <c r="K48">
         <v>0</v>
       </c>
       <c r="L48">
@@ -2981,12 +2978,12 @@
         <v>2693</v>
       </c>
       <c r="H49" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
       </c>
       <c r="J49">
-        <v>0</v>
-      </c>
-      <c r="K49">
         <v>0</v>
       </c>
       <c r="L49">
@@ -3031,12 +3028,12 @@
         <v>2088</v>
       </c>
       <c r="H50" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
       </c>
       <c r="J50">
-        <v>0</v>
-      </c>
-      <c r="K50">
         <v>0</v>
       </c>
       <c r="L50">
@@ -3081,12 +3078,12 @@
         <v>2095</v>
       </c>
       <c r="H51" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
       </c>
       <c r="J51">
-        <v>0</v>
-      </c>
-      <c r="K51">
         <v>0</v>
       </c>
       <c r="L51">
@@ -3131,12 +3128,12 @@
         <v>3020</v>
       </c>
       <c r="H52" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
       </c>
       <c r="J52">
-        <v>0</v>
-      </c>
-      <c r="K52">
         <v>0</v>
       </c>
       <c r="L52">
@@ -3181,12 +3178,12 @@
         <v>3682</v>
       </c>
       <c r="H53" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
       </c>
       <c r="J53">
-        <v>0</v>
-      </c>
-      <c r="K53">
         <v>0</v>
       </c>
       <c r="L53">
@@ -3231,12 +3228,12 @@
         <v>3686</v>
       </c>
       <c r="H54" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
       </c>
       <c r="J54">
-        <v>0</v>
-      </c>
-      <c r="K54">
         <v>0</v>
       </c>
       <c r="L54">
@@ -3281,12 +3278,12 @@
         <v>2267</v>
       </c>
       <c r="H55" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
       </c>
       <c r="J55">
-        <v>0</v>
-      </c>
-      <c r="K55">
         <v>0</v>
       </c>
       <c r="L55">
@@ -3331,12 +3328,12 @@
         <v>1520</v>
       </c>
       <c r="H56" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
       </c>
       <c r="J56">
-        <v>0</v>
-      </c>
-      <c r="K56">
         <v>0</v>
       </c>
       <c r="L56">
@@ -3381,12 +3378,12 @@
         <v>4870</v>
       </c>
       <c r="H57" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
       </c>
       <c r="J57">
-        <v>0</v>
-      </c>
-      <c r="K57">
         <v>0</v>
       </c>
       <c r="L57">
@@ -3431,12 +3428,12 @@
         <v>13583</v>
       </c>
       <c r="H58" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
       </c>
       <c r="J58">
-        <v>0</v>
-      </c>
-      <c r="K58">
         <v>0</v>
       </c>
       <c r="L58">
@@ -3481,12 +3478,12 @@
         <v>11703</v>
       </c>
       <c r="H59" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
       </c>
       <c r="J59">
-        <v>0</v>
-      </c>
-      <c r="K59">
         <v>0</v>
       </c>
       <c r="L59">
@@ -3531,12 +3528,12 @@
         <v>1676</v>
       </c>
       <c r="H60" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
       </c>
       <c r="J60">
-        <v>0</v>
-      </c>
-      <c r="K60">
         <v>0</v>
       </c>
       <c r="L60">
@@ -3581,12 +3578,12 @@
         <v>3537</v>
       </c>
       <c r="H61" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
       </c>
       <c r="J61">
-        <v>0</v>
-      </c>
-      <c r="K61">
         <v>0</v>
       </c>
       <c r="L61">
@@ -3631,12 +3628,12 @@
         <v>8493</v>
       </c>
       <c r="H62" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
       </c>
       <c r="J62">
-        <v>0</v>
-      </c>
-      <c r="K62">
         <v>0</v>
       </c>
       <c r="L62">
@@ -3681,12 +3678,12 @@
         <v>6365</v>
       </c>
       <c r="H63" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
       </c>
       <c r="J63">
-        <v>0</v>
-      </c>
-      <c r="K63">
         <v>0</v>
       </c>
       <c r="L63">
@@ -3731,12 +3728,12 @@
         <v>6122</v>
       </c>
       <c r="H64" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
       </c>
       <c r="J64">
-        <v>0</v>
-      </c>
-      <c r="K64">
         <v>0</v>
       </c>
       <c r="L64">
@@ -3781,12 +3778,12 @@
         <v>7225</v>
       </c>
       <c r="H65" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
       </c>
       <c r="J65">
-        <v>0</v>
-      </c>
-      <c r="K65">
         <v>0</v>
       </c>
       <c r="L65">
@@ -3831,12 +3828,12 @@
         <v>3872</v>
       </c>
       <c r="H66" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
       </c>
       <c r="J66">
-        <v>0</v>
-      </c>
-      <c r="K66">
         <v>0</v>
       </c>
       <c r="L66">
@@ -3881,12 +3878,12 @@
         <v>19891</v>
       </c>
       <c r="H67" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
       </c>
       <c r="J67">
-        <v>0</v>
-      </c>
-      <c r="K67">
         <v>0</v>
       </c>
       <c r="L67">
@@ -3931,12 +3928,12 @@
         <v>11590</v>
       </c>
       <c r="H68" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
       </c>
       <c r="J68">
-        <v>0</v>
-      </c>
-      <c r="K68">
         <v>0</v>
       </c>
       <c r="L68">
@@ -3981,12 +3978,12 @@
         <v>13473</v>
       </c>
       <c r="H69" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
       </c>
       <c r="J69">
-        <v>0</v>
-      </c>
-      <c r="K69">
         <v>0</v>
       </c>
       <c r="L69">
@@ -4031,12 +4028,12 @@
         <v>12799</v>
       </c>
       <c r="H70" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
       </c>
       <c r="J70">
-        <v>0</v>
-      </c>
-      <c r="K70">
         <v>0</v>
       </c>
       <c r="L70">
@@ -4081,12 +4078,12 @@
         <v>7907</v>
       </c>
       <c r="H71" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
       </c>
       <c r="J71">
-        <v>0</v>
-      </c>
-      <c r="K71">
         <v>0</v>
       </c>
       <c r="L71">
@@ -4131,12 +4128,12 @@
         <v>13974</v>
       </c>
       <c r="H72" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
       </c>
       <c r="J72">
-        <v>0</v>
-      </c>
-      <c r="K72">
         <v>0</v>
       </c>
       <c r="L72">
@@ -4181,12 +4178,12 @@
         <v>8372</v>
       </c>
       <c r="H73" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
       </c>
       <c r="J73">
-        <v>0</v>
-      </c>
-      <c r="K73">
         <v>0</v>
       </c>
       <c r="L73">
@@ -4231,12 +4228,12 @@
         <v>10269</v>
       </c>
       <c r="H74" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="I74">
+        <v>0</v>
       </c>
       <c r="J74">
-        <v>0</v>
-      </c>
-      <c r="K74">
         <v>0</v>
       </c>
       <c r="L74">
@@ -4281,12 +4278,12 @@
         <v>5910</v>
       </c>
       <c r="H75" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="I75">
+        <v>0</v>
       </c>
       <c r="J75">
-        <v>0</v>
-      </c>
-      <c r="K75">
         <v>0</v>
       </c>
       <c r="L75">
@@ -4331,12 +4328,12 @@
         <v>7135</v>
       </c>
       <c r="H76" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="I76">
+        <v>0</v>
       </c>
       <c r="J76">
-        <v>0</v>
-      </c>
-      <c r="K76">
         <v>0</v>
       </c>
       <c r="L76">
@@ -4381,12 +4378,12 @@
         <v>12798</v>
       </c>
       <c r="H77" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
       </c>
       <c r="J77">
-        <v>0</v>
-      </c>
-      <c r="K77">
         <v>0</v>
       </c>
       <c r="L77">
@@ -4431,12 +4428,12 @@
         <v>6467</v>
       </c>
       <c r="H78" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="I78">
+        <v>0</v>
       </c>
       <c r="J78">
-        <v>0</v>
-      </c>
-      <c r="K78">
         <v>0</v>
       </c>
       <c r="L78">
@@ -4481,12 +4478,12 @@
         <v>15894</v>
       </c>
       <c r="H79" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="I79">
+        <v>0</v>
       </c>
       <c r="J79">
-        <v>0</v>
-      </c>
-      <c r="K79">
         <v>0</v>
       </c>
       <c r="L79">
@@ -4531,12 +4528,12 @@
         <v>13013</v>
       </c>
       <c r="H80" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="I80">
+        <v>0</v>
       </c>
       <c r="J80">
-        <v>0</v>
-      </c>
-      <c r="K80">
         <v>0</v>
       </c>
       <c r="L80">
@@ -4581,12 +4578,12 @@
         <v>9608</v>
       </c>
       <c r="H81" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="I81">
+        <v>0</v>
       </c>
       <c r="J81">
-        <v>0</v>
-      </c>
-      <c r="K81">
         <v>0</v>
       </c>
       <c r="L81">
@@ -4631,12 +4628,12 @@
         <v>11435</v>
       </c>
       <c r="H82" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="I82">
+        <v>0</v>
       </c>
       <c r="J82">
-        <v>0</v>
-      </c>
-      <c r="K82">
         <v>0</v>
       </c>
       <c r="L82">
@@ -4681,12 +4678,12 @@
         <v>19308</v>
       </c>
       <c r="H83" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="I83">
+        <v>0</v>
       </c>
       <c r="J83">
-        <v>0</v>
-      </c>
-      <c r="K83">
         <v>0</v>
       </c>
       <c r="L83">
@@ -4731,12 +4728,12 @@
         <v>17977</v>
       </c>
       <c r="H84" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="I84">
+        <v>0</v>
       </c>
       <c r="J84">
-        <v>0</v>
-      </c>
-      <c r="K84">
         <v>0</v>
       </c>
       <c r="L84">
@@ -4781,12 +4778,12 @@
         <v>11619</v>
       </c>
       <c r="H85" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="I85">
+        <v>0</v>
       </c>
       <c r="J85">
-        <v>0</v>
-      </c>
-      <c r="K85">
         <v>0</v>
       </c>
       <c r="L85">
@@ -4831,12 +4828,12 @@
         <v>10034</v>
       </c>
       <c r="H86" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="I86">
+        <v>0</v>
       </c>
       <c r="J86">
-        <v>0</v>
-      </c>
-      <c r="K86">
         <v>0</v>
       </c>
       <c r="L86">
@@ -4881,12 +4878,12 @@
         <v>19359</v>
       </c>
       <c r="H87" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="I87">
+        <v>0</v>
       </c>
       <c r="J87">
-        <v>0</v>
-      </c>
-      <c r="K87">
         <v>0</v>
       </c>
       <c r="L87">
@@ -4931,12 +4928,12 @@
         <v>17057</v>
       </c>
       <c r="H88" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="I88">
+        <v>0</v>
       </c>
       <c r="J88">
-        <v>0</v>
-      </c>
-      <c r="K88">
         <v>0</v>
       </c>
       <c r="L88">
@@ -4981,12 +4978,12 @@
         <v>13998</v>
       </c>
       <c r="H89" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="I89">
+        <v>0</v>
       </c>
       <c r="J89">
-        <v>0</v>
-      </c>
-      <c r="K89">
         <v>0</v>
       </c>
       <c r="L89">
@@ -5031,12 +5028,12 @@
         <v>15030</v>
       </c>
       <c r="H90" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="I90">
+        <v>0</v>
       </c>
       <c r="J90">
-        <v>0</v>
-      </c>
-      <c r="K90">
         <v>0</v>
       </c>
       <c r="L90">
@@ -5081,12 +5078,12 @@
         <v>19560</v>
       </c>
       <c r="H91" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="I91">
+        <v>0</v>
       </c>
       <c r="J91">
-        <v>0</v>
-      </c>
-      <c r="K91">
         <v>0</v>
       </c>
       <c r="L91">
@@ -5131,12 +5128,12 @@
         <v>17258</v>
       </c>
       <c r="H92" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="I92">
+        <v>0</v>
       </c>
       <c r="J92">
-        <v>0</v>
-      </c>
-      <c r="K92">
         <v>0</v>
       </c>
       <c r="L92">
@@ -5181,12 +5178,12 @@
         <v>10429</v>
       </c>
       <c r="H93" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="I93">
+        <v>0</v>
       </c>
       <c r="J93">
-        <v>0</v>
-      </c>
-      <c r="K93">
         <v>0</v>
       </c>
       <c r="L93">
@@ -5231,12 +5228,12 @@
         <v>9922</v>
       </c>
       <c r="H94" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="I94">
+        <v>0</v>
       </c>
       <c r="J94">
-        <v>0</v>
-      </c>
-      <c r="K94">
         <v>0</v>
       </c>
       <c r="L94">
@@ -5281,12 +5278,12 @@
         <v>8446</v>
       </c>
       <c r="H95" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="I95">
+        <v>0</v>
       </c>
       <c r="J95">
-        <v>0</v>
-      </c>
-      <c r="K95">
         <v>0</v>
       </c>
       <c r="L95">
@@ -5331,12 +5328,12 @@
         <v>18897</v>
       </c>
       <c r="H96" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="I96">
+        <v>0</v>
       </c>
       <c r="J96">
-        <v>0</v>
-      </c>
-      <c r="K96">
         <v>0</v>
       </c>
       <c r="L96">
@@ -5381,12 +5378,12 @@
         <v>10342</v>
       </c>
       <c r="H97" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="I97">
+        <v>0</v>
       </c>
       <c r="J97">
-        <v>0</v>
-      </c>
-      <c r="K97">
         <v>0</v>
       </c>
       <c r="L97">
@@ -5431,12 +5428,12 @@
         <v>19051</v>
       </c>
       <c r="H98" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="I98">
+        <v>0</v>
       </c>
       <c r="J98">
-        <v>0</v>
-      </c>
-      <c r="K98">
         <v>0</v>
       </c>
       <c r="L98">
@@ -5481,12 +5478,12 @@
         <v>15102</v>
       </c>
       <c r="H99" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="I99">
+        <v>0</v>
       </c>
       <c r="J99">
-        <v>0</v>
-      </c>
-      <c r="K99">
         <v>0</v>
       </c>
       <c r="L99">
@@ -5531,12 +5528,12 @@
         <v>5309</v>
       </c>
       <c r="H100" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="I100">
+        <v>0</v>
       </c>
       <c r="J100">
-        <v>0</v>
-      </c>
-      <c r="K100">
         <v>0</v>
       </c>
       <c r="L100">
@@ -5581,12 +5578,12 @@
         <v>10158</v>
       </c>
       <c r="H101" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="I101">
+        <v>0</v>
       </c>
       <c r="J101">
-        <v>0</v>
-      </c>
-      <c r="K101">
         <v>0</v>
       </c>
       <c r="L101">
@@ -6189,52 +6186,52 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -6255,13 +6252,13 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>15</v>
@@ -6269,57 +6266,57 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4">
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6">
         <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -6337,34 +6334,34 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>15</v>
@@ -6390,7 +6387,7 @@
         <v>29.849686</v>
       </c>
       <c r="K2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>